<commit_message>
versjon av dokumenter som er oversendt til Kjeller V.
</commit_message>
<xml_diff>
--- a/doc/actions lastmåler.xlsx
+++ b/doc/actions lastmåler.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.rune.herheim\Dropbox (Lillebakk)\Lillebakk Team\herheim\Documents\customers\kjeller vindteknikk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.rune.herheim\Dropbox (Lillebakk)\Lillebakk Team\herheim\Documents\GitHub\LE_NB_IOT_CONTROLLER\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="138">
   <si>
     <t>Action ID</t>
   </si>
@@ -397,9 +397,6 @@
     <t>Kjeller har dårlig erfaring med HBM lastcelle (ustabil og dyr)</t>
   </si>
   <si>
-    <t>Få pris på lastcelle som brukes I dagens løsning og den som KV har gode erfaringer med (Vishaypg). Også sjekke den som sitter I 1 tonns versjonen.</t>
-  </si>
-  <si>
     <t>Lastcelle + maskinering for dyrt I dagens kalkyler.</t>
   </si>
   <si>
@@ -498,6 +495,10 @@
   <si>
     <t>Gode erfaringer med produkt til Fugro (Ola)
 Frode sjekker med Thomas(?) hos PartnerPlast. Det kan være at 50 enheter er for lite til at det lønner seg. Mål om å finne knekkpunktet der plast tar over for alu. Ev definere concept3 som plastinnkapsling, og concept2 som alu.</t>
+  </si>
+  <si>
+    <t>Få pris på lastcelle som brukes I dagens løsning og den som KV har gode erfaringer med (Vishaypg). Også sjekke den som sitter I 1 tonns versjonen.
+Estimert pris fra KV er ~8k. Bruker denne prisen I estimat for concept2.</t>
   </si>
 </sst>
 </file>
@@ -933,8 +934,8 @@
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -982,10 +983,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -1009,11 +1013,13 @@
       </c>
       <c r="J2"/>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1037,9 +1043,12 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>17</v>
@@ -1069,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>19</v>
@@ -1177,9 +1186,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>30</v>
@@ -1265,7 +1277,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>43</v>
@@ -1286,11 +1298,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
@@ -1349,7 +1363,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>52</v>
@@ -1374,10 +1388,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C16" s="13" t="s">
         <v>55</v>
       </c>
@@ -1403,10 +1420,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C17" s="13" t="s">
         <v>56</v>
       </c>
@@ -1430,11 +1450,13 @@
       </c>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" s="6" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="C18" s="13" t="s">
         <v>57</v>
       </c>
@@ -1463,7 +1485,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>58</v>
@@ -1486,9 +1508,12 @@
       <c r="I19" s="8"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>59</v>
@@ -1518,7 +1543,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>61</v>
@@ -1541,9 +1566,12 @@
       <c r="I21" s="8"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>110</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>62</v>
@@ -1626,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>92</v>
@@ -1654,7 +1682,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>74</v>
@@ -1682,7 +1710,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>76</v>
@@ -1712,7 +1740,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>78</v>
@@ -1733,9 +1761,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>79</v>
@@ -1804,7 +1835,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>85</v>
@@ -1828,12 +1859,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>86</v>
@@ -1862,7 +1893,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>87</v>
@@ -1891,7 +1922,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>90</v>
@@ -1920,7 +1951,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>93</v>
@@ -1946,7 +1977,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>94</v>
@@ -1972,7 +2003,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>96</v>
@@ -1996,7 +2027,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2025,7 +2056,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2033,7 +2064,7 @@
         <v>103</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>10</v>
@@ -2062,7 +2093,7 @@
         <v>103</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>10</v>
@@ -2080,7 +2111,7 @@
         <v>28</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
@@ -2109,10 +2140,10 @@
         <v>28</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2138,10 +2169,10 @@
         <v>21</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2167,7 +2198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2189,11 +2220,11 @@
       <c r="G45" t="s">
         <v>50</v>
       </c>
-      <c r="H45" t="s">
-        <v>28</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>108</v>
+      <c r="H45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
@@ -2204,7 +2235,7 @@
         <v>103</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>10</v>
@@ -2222,7 +2253,7 @@
         <v>28</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2230,10 +2261,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="16" t="s">
         <v>111</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>75</v>
@@ -2251,18 +2282,18 @@
         <v>28</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>10</v>
@@ -2280,7 +2311,7 @@
         <v>28</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2291,7 +2322,7 @@
         <v>103</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>75</v>
@@ -2314,10 +2345,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>75</v>
@@ -2340,10 +2371,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>10</v>
@@ -2366,10 +2397,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>10</v>
@@ -2387,7 +2418,7 @@
         <v>28</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2398,7 +2429,7 @@
         <v>103</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D53" s="19" t="s">
         <v>10</v>
@@ -2416,7 +2447,7 @@
         <v>28</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2424,10 +2455,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>10</v>
@@ -2445,7 +2476,7 @@
         <v>28</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2453,10 +2484,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>10</v>
@@ -2474,24 +2505,24 @@
         <v>28</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F56" t="s">
         <v>33</v>
@@ -2503,7 +2534,7 @@
         <v>28</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -2511,10 +2542,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>10</v>
@@ -2532,7 +2563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="89.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2540,7 +2571,7 @@
         <v>103</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>10</v>
@@ -2558,7 +2589,7 @@
         <v>28</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -2566,10 +2597,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>10</v>
@@ -2587,18 +2618,18 @@
         <v>28</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>75</v>
@@ -2616,7 +2647,7 @@
         <v>28</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -2876,12 +2907,6 @@
         <filter val="JRH"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="7">
-      <filters blank="1">
-        <filter val="ongoing"/>
-        <filter val="open"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A5:J108">
       <sortCondition ref="A1:A108"/>
     </sortState>

</xml_diff>